<commit_message>
add gaussian blur before apply threshold and apply morphology after
</commit_message>
<xml_diff>
--- a/ProcessoSeletivo.xlsx
+++ b/ProcessoSeletivo.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
@@ -1307,32 +1307,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>indigena</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1762,6 +1762,123 @@
         </is>
       </c>
       <c r="W12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Rodrigo Souza Santos</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
update to register answers
</commit_message>
<xml_diff>
--- a/ProcessoSeletivo.xlsx
+++ b/ProcessoSeletivo.xlsx
@@ -1074,112 +1074,112 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>a</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>c</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>c</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>d</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>b</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>c</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>d</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>b</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>d</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>d</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>b</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>c</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>d</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>c</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>b</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>c</t>
         </is>
       </c>
     </row>
@@ -2630,7 +2630,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>

</xml_diff>

<commit_message>
feat debug by args
</commit_message>
<xml_diff>
--- a/ProcessoSeletivo.xlsx
+++ b/ProcessoSeletivo.xlsx
@@ -501,7 +501,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -511,97 +511,97 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>d</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
         <is>
           <t>e</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
         <is>
           <t>d</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>b</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">

</xml_diff>

<commit_message>
feat: select test by excel
</commit_message>
<xml_diff>
--- a/ProcessoSeletivo.xlsx
+++ b/ProcessoSeletivo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\son5ct\Desktop\Projects\Ets-SPP (copy)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D57922-3C3C-4131-B9FC-9E5FBC8C13DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38F4658-93F4-46E1-BC4E-AD429DD03D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="4335" windowWidth="21600" windowHeight="11580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registros" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="1522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="1522">
   <si>
     <t>Nome</t>
   </si>
@@ -4796,7 +4796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4844,6 +4844,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5128,8 +5134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1506"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5211,231 +5217,105 @@
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>4</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>1517</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>1519</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>1521</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>1520</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>1517</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>1519</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>1521</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>1519</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>1519</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>1517</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>1521</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>1520</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>1517</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>1521</v>
-      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="18"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>1517</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>1518</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>1519</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>1521</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>1517</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>1518</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>1519</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>1521</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>1517</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="U3" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>1521</v>
-      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="18"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="8"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="18"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>1517</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>1518</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>1518</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>1519</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>1521</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>1517</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>1518</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>1519</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>1521</v>
-      </c>
-      <c r="R5" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>1517</v>
-      </c>
-      <c r="T5" s="15" t="s">
-        <v>1518</v>
-      </c>
-      <c r="U5" s="15" t="s">
-        <v>1520</v>
-      </c>
-      <c r="V5" s="16" t="s">
-        <v>1521</v>
-      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="18"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -44767,8 +44647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:A21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>